<commit_message>
paul want to try to creat the schedule
</commit_message>
<xml_diff>
--- a/2020-2021（1）Annee2.xlsx
+++ b/2020-2021（1）Annee2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\课程安排\2020-2021（1）\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\python\auto_chat_robot\wechat_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC9188F-D85F-4AE8-AE36-7B8CA253DD25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27735" windowHeight="11790"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3161,7 +3162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="hh:mm"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
@@ -3850,404 +3851,348 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4282,7 +4227,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="LOGO_GEA_blanc"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="LOGO_GEA_blanc">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4350,7 +4301,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 4" descr="logoCAUC"/>
+        <xdr:cNvPr id="4" name="Picture 4" descr="logoCAUC">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4668,30 +4625,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.25" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="42" t="s">
         <v>16</v>
@@ -4706,7 +4663,7 @@
       <c r="J1" s="42"/>
       <c r="K1" s="43"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="44"/>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -4719,7 +4676,7 @@
       <c r="J2" s="45"/>
       <c r="K2" s="45"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
         <v>17</v>
       </c>
@@ -4734,7 +4691,7 @@
       <c r="J3" s="47"/>
       <c r="K3" s="47"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>18</v>
       </c>
@@ -4749,7 +4706,7 @@
       <c r="J4" s="49"/>
       <c r="K4" s="49"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>14</v>
       </c>
@@ -4764,7 +4721,7 @@
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36"/>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -4777,7 +4734,7 @@
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="34" t="s">
         <v>13</v>
@@ -4800,7 +4757,7 @@
       </c>
       <c r="K7" s="41"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0.33333333333333298</v>
       </c>
@@ -4815,7 +4772,7 @@
       <c r="J8" s="38"/>
       <c r="K8" s="40"/>
     </row>
-    <row r="9" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="16" t="s">
         <v>19</v>
@@ -4838,7 +4795,7 @@
       </c>
       <c r="K9" s="57"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -4853,7 +4810,7 @@
       <c r="J10" s="58"/>
       <c r="K10" s="59"/>
     </row>
-    <row r="11" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21"/>
@@ -4866,7 +4823,7 @@
       <c r="J11" s="60"/>
       <c r="K11" s="61"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4881,22 +4838,22 @@
       <c r="J12" s="71"/>
       <c r="K12" s="72"/>
     </row>
-    <row r="13" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="99" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="98" t="s">
+      <c r="G13" s="99" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="56" t="s">
@@ -4908,35 +4865,35 @@
       </c>
       <c r="K13" s="62"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="102"/>
-      <c r="C14" s="99"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="100"/>
       <c r="D14" s="18"/>
       <c r="E14" s="19"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="99"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="100"/>
       <c r="H14" s="58"/>
       <c r="I14" s="87"/>
       <c r="J14" s="18"/>
       <c r="K14" s="63"/>
     </row>
-    <row r="15" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="100"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="101"/>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="100"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="101"/>
       <c r="H15" s="60"/>
       <c r="I15" s="88"/>
       <c r="J15" s="20"/>
       <c r="K15" s="64"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
@@ -4951,7 +4908,7 @@
       <c r="J16" s="71"/>
       <c r="K16" s="72"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="93"/>
       <c r="C17" s="94"/>
@@ -4964,33 +4921,33 @@
       <c r="J17" s="93"/>
       <c r="K17" s="95"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="104"/>
       <c r="B18" s="89"/>
-      <c r="C18" s="96"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="89"/>
-      <c r="E18" s="96"/>
+      <c r="E18" s="102"/>
       <c r="F18" s="89"/>
-      <c r="G18" s="96"/>
+      <c r="G18" s="102"/>
       <c r="H18" s="89"/>
-      <c r="I18" s="96"/>
+      <c r="I18" s="102"/>
       <c r="J18" s="89"/>
       <c r="K18" s="90"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="105"/>
       <c r="B19" s="91"/>
-      <c r="C19" s="97"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="91"/>
-      <c r="E19" s="97"/>
+      <c r="E19" s="103"/>
       <c r="F19" s="91"/>
-      <c r="G19" s="97"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="91"/>
-      <c r="I19" s="97"/>
+      <c r="I19" s="103"/>
       <c r="J19" s="91"/>
       <c r="K19" s="92"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>0.5625</v>
       </c>
@@ -5005,66 +4962,66 @@
       <c r="J20" s="71"/>
       <c r="K20" s="72"/>
     </row>
-    <row r="21" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="132" t="s">
+      <c r="E21" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="129" t="s">
+      <c r="H21" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="126" t="s">
+      <c r="I21" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="143" t="s">
+      <c r="J21" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="144"/>
+      <c r="K21" s="127"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="99"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="107"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="130"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="145"/>
-      <c r="K22" s="146"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="133"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="129"/>
     </row>
-    <row r="23" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="B23" s="103"/>
-      <c r="C23" s="100"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="108"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="131"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="147"/>
-      <c r="K23" s="148"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="101"/>
+      <c r="H23" s="137"/>
+      <c r="I23" s="134"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="131"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -5076,15 +5033,15 @@
       <c r="G24" s="73"/>
       <c r="H24" s="71"/>
       <c r="I24" s="73"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="142"/>
+      <c r="J24" s="147"/>
+      <c r="K24" s="148"/>
     </row>
-    <row r="25" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="135" t="s">
+      <c r="B25" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="136"/>
+      <c r="C25" s="142"/>
       <c r="D25" s="50" t="s">
         <v>25</v>
       </c>
@@ -5100,12 +5057,12 @@
       <c r="J25" s="74"/>
       <c r="K25" s="75"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="137"/>
-      <c r="C26" s="138"/>
+      <c r="B26" s="143"/>
+      <c r="C26" s="144"/>
       <c r="D26" s="52"/>
       <c r="E26" s="53"/>
       <c r="F26" s="52"/>
@@ -5115,10 +5072,10 @@
       <c r="J26" s="76"/>
       <c r="K26" s="77"/>
     </row>
-    <row r="27" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="139"/>
-      <c r="C27" s="140"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="146"/>
       <c r="D27" s="54"/>
       <c r="E27" s="55"/>
       <c r="F27" s="54"/>
@@ -5128,7 +5085,7 @@
       <c r="J27" s="78"/>
       <c r="K27" s="79"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>1</v>
       </c>
@@ -5143,7 +5100,7 @@
       <c r="J28" s="71"/>
       <c r="K28" s="72"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="93"/>
       <c r="C29" s="94"/>
@@ -5156,7 +5113,7 @@
       <c r="J29" s="93"/>
       <c r="K29" s="95"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>0.77083333333333304</v>
       </c>
@@ -5171,7 +5128,7 @@
       <c r="J30" s="71"/>
       <c r="K30" s="72"/>
     </row>
-    <row r="31" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="74"/>
       <c r="C31" s="113"/>
@@ -5188,7 +5145,7 @@
       <c r="J31" s="119"/>
       <c r="K31" s="120"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>0</v>
       </c>
@@ -5203,7 +5160,7 @@
       <c r="J32" s="121"/>
       <c r="K32" s="122"/>
     </row>
-    <row r="33" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="78"/>
       <c r="C33" s="115"/>
@@ -5216,7 +5173,7 @@
       <c r="J33" s="123"/>
       <c r="K33" s="124"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>0.83680555555555503</v>
       </c>
@@ -5231,7 +5188,7 @@
       <c r="J34" s="109"/>
       <c r="K34" s="111"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="112" t="s">
         <v>28</v>
       </c>
@@ -5246,7 +5203,7 @@
       <c r="J35" s="112"/>
       <c r="K35" s="14"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>15</v>
       </c>
@@ -5262,107 +5219,6 @@
       <c r="K36" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="J21:K23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="D25:E27"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="B31:C33"/>
-    <mergeCell ref="F31:G33"/>
-    <mergeCell ref="J31:K33"/>
-    <mergeCell ref="H31:I33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="H9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="J13:K15"/>
-    <mergeCell ref="D31:E33"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="J25:K27"/>
-    <mergeCell ref="H25:I27"/>
-    <mergeCell ref="F25:G27"/>
-    <mergeCell ref="H13:I15"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B9:C11"/>
-    <mergeCell ref="D9:E11"/>
-    <mergeCell ref="F9:G11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>